<commit_message>
casi lsito, para una factura
</commit_message>
<xml_diff>
--- a/campos.xlsx
+++ b/campos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Desktop\Program_Facturación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6F45293-E3FA-4B50-9EB5-8398B5478C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC356E2-296C-4ECD-BFBE-3C0813015BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{B067860B-7991-4F3F-B7C1-A4E8871595C2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{B067860B-7991-4F3F-B7C1-A4E8871595C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -568,9 +560,6 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -585,21 +574,24 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -916,13 +908,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5062CB8A-FA6F-4F7C-9127-EB1481887452}">
   <dimension ref="A2:AG9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:33" ht="306" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" ht="290.39999999999998" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1023,7 +1015,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" ht="69" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -1124,7 +1116,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>39</v>
       </c>
@@ -1225,7 +1217,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>42</v>
       </c>
@@ -1326,7 +1318,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:33" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>43</v>
       </c>
@@ -1427,192 +1419,192 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:33" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="1:33" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="J7" s="16" t="s">
+      <c r="J7" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="K7" s="16" t="s">
+      <c r="K7" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="L7" s="16" t="s">
+      <c r="L7" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="M7" s="16" t="s">
+      <c r="M7" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="N7" s="16" t="s">
+      <c r="N7" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="O7" s="16" t="s">
+      <c r="O7" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="P7" s="16" t="s">
+      <c r="P7" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="Q7" s="16" t="s">
+      <c r="Q7" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="R7" s="16" t="s">
+      <c r="R7" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="S7" s="16" t="s">
+      <c r="S7" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="T7" s="19" t="s">
+      <c r="T7" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="U7" s="16" t="s">
+      <c r="U7" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="V7" s="16" t="s">
+      <c r="V7" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="W7" s="16" t="s">
+      <c r="W7" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="X7" s="16" t="s">
+      <c r="X7" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="Y7" s="16" t="s">
+      <c r="Y7" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="Z7" s="16" t="s">
+      <c r="Z7" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="AA7" s="16" t="s">
+      <c r="AA7" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="AB7" s="17" t="s">
+      <c r="AB7" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="AC7" s="17" t="s">
+      <c r="AC7" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="AD7" s="17" t="s">
+      <c r="AD7" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="AE7" s="17" t="s">
+      <c r="AE7" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="AF7" s="17" t="s">
+      <c r="AF7" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="AG7" s="17" t="s">
+      <c r="AG7" s="16" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:33" ht="288.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="19" t="s">
+    <row r="8" spans="1:33" ht="229.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="28"/>
+      <c r="B8" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="19" t="s">
+      <c r="C8" s="19"/>
+      <c r="D8" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19" t="s">
+      <c r="E8" s="20"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="L8" s="19" t="s">
+      <c r="L8" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="M8" s="19" t="s">
+      <c r="M8" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="23"/>
-      <c r="V8" s="23"/>
-      <c r="W8" s="23"/>
-      <c r="X8" s="19"/>
-      <c r="Y8" s="19" t="s">
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="21"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="21"/>
+      <c r="U8" s="21"/>
+      <c r="V8" s="21"/>
+      <c r="W8" s="21"/>
+      <c r="X8" s="18"/>
+      <c r="Y8" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="Z8" s="19"/>
-      <c r="AA8" s="19" t="s">
+      <c r="Z8" s="18"/>
+      <c r="AA8" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="AB8" s="23"/>
-      <c r="AC8" s="23"/>
-      <c r="AD8" s="23"/>
-      <c r="AE8" s="23"/>
-      <c r="AF8" s="23"/>
-      <c r="AG8" s="23"/>
+      <c r="AB8" s="21"/>
+      <c r="AC8" s="21"/>
+      <c r="AD8" s="21"/>
+      <c r="AE8" s="21"/>
+      <c r="AF8" s="21"/>
+      <c r="AG8" s="21"/>
     </row>
-    <row r="9" spans="1:33" ht="36.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="19" t="s">
+    <row r="9" spans="1:33" ht="35.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="29"/>
+      <c r="B9" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="27"/>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="27"/>
-      <c r="S9" s="27"/>
-      <c r="T9" s="27"/>
-      <c r="U9" s="27"/>
-      <c r="V9" s="27"/>
-      <c r="W9" s="27"/>
-      <c r="X9" s="27"/>
-      <c r="Y9" s="27"/>
-      <c r="Z9" s="27"/>
-      <c r="AA9" s="27"/>
-      <c r="AB9" s="27"/>
-      <c r="AC9" s="27"/>
-      <c r="AD9" s="27"/>
-      <c r="AE9" s="27"/>
-      <c r="AF9" s="27"/>
-      <c r="AG9" s="27"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="26"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="24"/>
+      <c r="V9" s="24"/>
+      <c r="W9" s="24"/>
+      <c r="X9" s="24"/>
+      <c r="Y9" s="24"/>
+      <c r="Z9" s="24"/>
+      <c r="AA9" s="24"/>
+      <c r="AB9" s="24"/>
+      <c r="AC9" s="24"/>
+      <c r="AD9" s="24"/>
+      <c r="AE9" s="24"/>
+      <c r="AF9" s="24"/>
+      <c r="AG9" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>